<commit_message>
add requirements.txt and README.md
</commit_message>
<xml_diff>
--- a/entrega/planillas/OCL_huffman.xlsx
+++ b/entrega/planillas/OCL_huffman.xlsx
@@ -3880,10 +3880,10 @@
         <v>0.9934804592025525</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0006585121154785156</v>
+        <v>0.0004668235778808594</v>
       </c>
       <c r="H2" t="n">
-        <v>0.006209135055541992</v>
+        <v>0.00756382942199707</v>
       </c>
     </row>
   </sheetData>

</xml_diff>